<commit_message>
Added new end point getAvgFlightInTime
</commit_message>
<xml_diff>
--- a/static/uploads/SaudiCaterers_Data_template_-_Copy.xlsx
+++ b/static/uploads/SaudiCaterers_Data_template_-_Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balac\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D5582A-439D-450E-9F12-B1B18CACC929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E84E134-2FC6-4FC0-8932-782DEE038001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{B2BCA890-1C30-4CAB-956F-81534F26E792}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B2BCA890-1C30-4CAB-956F-81534F26E792}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Mapping" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="117">
   <si>
     <t>Item</t>
   </si>
@@ -389,6 +389,12 @@
   </si>
   <si>
     <t>Sweet Dish</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Latitude</t>
   </si>
 </sst>
 </file>
@@ -430,11 +436,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -930,10 +935,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9AB7ADB-D63E-4A81-8C89-010E679DB448}">
-  <dimension ref="A1:Q44"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,7 +960,7 @@
     <col min="16" max="16" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1007,8 +1012,14 @@
       <c r="Q1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" t="s">
+        <v>115</v>
+      </c>
+      <c r="S1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1057,8 +1068,14 @@
       <c r="P2">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R2">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S2">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1107,8 +1124,14 @@
       <c r="P3">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R3">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S3">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1157,8 +1180,14 @@
       <c r="P4">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S4">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1207,8 +1236,14 @@
       <c r="P5">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S5">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1257,8 +1292,14 @@
       <c r="P6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R6">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S6">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1307,8 +1348,14 @@
       <c r="P7">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S7">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1357,8 +1404,14 @@
       <c r="P8">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R8">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S8">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1407,8 +1460,14 @@
       <c r="P9">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R9">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S9">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1457,8 +1516,14 @@
       <c r="P10">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S10">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1507,8 +1572,14 @@
       <c r="P11">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R11">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S11">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1557,8 +1628,14 @@
       <c r="P12">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R12">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S12">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1607,8 +1684,14 @@
       <c r="P13">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R13">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S13">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1657,8 +1740,14 @@
       <c r="P14">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R14">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S14">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1707,8 +1796,14 @@
       <c r="P15">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R15">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S15">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1757,8 +1852,14 @@
       <c r="P16">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R16">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S16">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1807,8 +1908,14 @@
       <c r="P17">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R17">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S17">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1857,8 +1964,14 @@
       <c r="P18">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R18">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S18">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1907,8 +2020,14 @@
       <c r="P19">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R19">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S19">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1957,8 +2076,14 @@
       <c r="P20">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R20">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S20">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -2007,8 +2132,14 @@
       <c r="P21">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R21">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S21">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -2057,8 +2188,14 @@
       <c r="P22">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R22">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S22">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -2107,8 +2244,14 @@
       <c r="P23">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R23">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S23">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -2157,8 +2300,14 @@
       <c r="P24">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R24">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S24">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -2207,8 +2356,14 @@
       <c r="P25">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R25">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S25">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -2257,8 +2412,14 @@
       <c r="P26">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R26">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S26">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2307,8 +2468,14 @@
       <c r="P27">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R27">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S27">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -2357,8 +2524,14 @@
       <c r="P28">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R28">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S28">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -2407,8 +2580,14 @@
       <c r="P29">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R29">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S29">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -2454,8 +2633,14 @@
       <c r="Q30">
         <v>107</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R30">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S30">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2501,8 +2686,14 @@
       <c r="Q31">
         <v>102</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R31">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S31">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2548,8 +2739,14 @@
       <c r="Q32">
         <v>109</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R32">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S32">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2595,8 +2792,14 @@
       <c r="Q33">
         <v>105</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R33">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S33">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -2642,8 +2845,14 @@
       <c r="Q34">
         <v>119</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R34">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S34">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -2689,8 +2898,14 @@
       <c r="Q35">
         <v>111</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R35">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S35">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -2736,8 +2951,14 @@
       <c r="Q36">
         <v>110</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R36">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S36">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -2789,8 +3010,14 @@
       <c r="Q37" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R37">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S37">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -2842,8 +3069,14 @@
       <c r="Q38" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R38">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S38">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -2895,8 +3128,14 @@
       <c r="Q39" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R39">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S39">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -2948,8 +3187,14 @@
       <c r="Q40" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R40">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S40">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -3001,8 +3246,14 @@
       <c r="Q41" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R41">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S41">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -3054,8 +3305,14 @@
       <c r="Q42" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R42">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S42">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -3107,8 +3364,14 @@
       <c r="Q43" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R43">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S43">
+        <v>15.666600000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -3159,6 +3422,12 @@
       </c>
       <c r="Q44" t="s">
         <v>79</v>
+      </c>
+      <c r="R44">
+        <v>10.111000000000001</v>
+      </c>
+      <c r="S44">
+        <v>15.666600000000001</v>
       </c>
     </row>
   </sheetData>
@@ -3238,7 +3507,7 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -3253,7 +3522,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B2">
@@ -3379,7 +3648,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>44562</v>
       </c>
       <c r="B2">
@@ -4093,9 +4362,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4243,19 +4515,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24C30AD3-505E-4898-9713-43C7CA44D311}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{019D34A0-B57A-4A21-AB0E-208939F6134E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4279,9 +4547,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{019D34A0-B57A-4A21-AB0E-208939F6134E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24C30AD3-505E-4898-9713-43C7CA44D311}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>